<commit_message>
SD card logging test working
SPI speed had to be decreased
</commit_message>
<xml_diff>
--- a/1-SystemDocs/Connections_Ports_Memory_spec.xlsx
+++ b/1-SystemDocs/Connections_Ports_Memory_spec.xlsx
@@ -15,14 +15,13 @@
     <sheet name="SPI ETH ESP32" sheetId="1" r:id="rId1"/>
     <sheet name="Pinout ETH DEEK" sheetId="2" r:id="rId2"/>
     <sheet name="JTAG conn" sheetId="3" r:id="rId3"/>
-    <sheet name="Hárok1" sheetId="10" r:id="rId4"/>
-    <sheet name="SD usage" sheetId="4" r:id="rId5"/>
-    <sheet name="UDP packets" sheetId="5" r:id="rId6"/>
-    <sheet name="UDP datagram definition" sheetId="6" r:id="rId7"/>
-    <sheet name="Message Types" sheetId="7" r:id="rId8"/>
-    <sheet name="ADC selection" sheetId="9" r:id="rId9"/>
-    <sheet name="Time budget" sheetId="11" r:id="rId10"/>
-    <sheet name="TO DO" sheetId="8" r:id="rId11"/>
+    <sheet name="SD usage" sheetId="4" r:id="rId4"/>
+    <sheet name="UDP packets" sheetId="5" r:id="rId5"/>
+    <sheet name="UDP datagram definition" sheetId="6" r:id="rId6"/>
+    <sheet name="Message Types" sheetId="7" r:id="rId7"/>
+    <sheet name="ADC selection" sheetId="9" r:id="rId8"/>
+    <sheet name="Time budget" sheetId="11" r:id="rId9"/>
+    <sheet name="TO DO" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -985,7 +984,7 @@
         <xdr:cNvPr id="2" name="Obrázok 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1280,7 +1279,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,7 +1313,12 @@
       <c r="H1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="J1" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>171</v>
+      </c>
       <c r="L1" t="s">
         <v>9</v>
       </c>
@@ -1338,12 +1342,6 @@
       </c>
       <c r="H2" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="J2" s="54" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1628,54 +1626,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>300</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -1710,7 +1660,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B6"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2102,18 +2052,6 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2229,7 +2167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -2292,7 +2230,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -2440,7 +2378,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H32"/>
   <sheetViews>
@@ -2841,7 +2779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -2946,4 +2884,52 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
VI and esp communication
</commit_message>
<xml_diff>
--- a/1-SystemDocs/Connections_Ports_Memory_spec.xlsx
+++ b/1-SystemDocs/Connections_Ports_Memory_spec.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="SPI ETH ESP32" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="181">
   <si>
     <t>ETH*</t>
   </si>
@@ -380,9 +380,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>6..9</t>
-  </si>
-  <si>
     <t>Analog input for sensor detection</t>
   </si>
   <si>
@@ -392,9 +389,6 @@
     <t>Baseline test for connected sensors</t>
   </si>
   <si>
-    <t>MESSAGE_TYPE</t>
-  </si>
-  <si>
     <t>Start trigger</t>
   </si>
   <si>
@@ -413,9 +407,6 @@
     <t>Built-in Test trigger</t>
   </si>
   <si>
-    <t>7..8</t>
-  </si>
-  <si>
     <t>ERROR CODE</t>
   </si>
   <si>
@@ -485,15 +476,6 @@
     <t>Sensor 12</t>
   </si>
   <si>
-    <t>10..13</t>
-  </si>
-  <si>
-    <t>14..18</t>
-  </si>
-  <si>
-    <t>50..53</t>
-  </si>
-  <si>
     <t>ADS114S08</t>
   </si>
   <si>
@@ -579,6 +561,27 @@
   </si>
   <si>
     <t>20MHz SPI</t>
+  </si>
+  <si>
+    <t>ANNOUNCEMENT announcing sensor unit is on network</t>
+  </si>
+  <si>
+    <t>COMMAND</t>
+  </si>
+  <si>
+    <t>5..8</t>
+  </si>
+  <si>
+    <t>9..12</t>
+  </si>
+  <si>
+    <t>13..17</t>
+  </si>
+  <si>
+    <t>49..52</t>
+  </si>
+  <si>
+    <t>6..7</t>
   </si>
 </sst>
 </file>
@@ -807,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -895,6 +898,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -993,7 +999,7 @@
         <xdr:cNvPr id="2" name="Obrázok 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1345,7 +1351,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
@@ -1369,7 +1375,7 @@
         <v>74</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -1452,7 +1458,7 @@
         <v>44</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="L4" s="1">
         <v>4</v>
@@ -1481,10 +1487,10 @@
         <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="L5" s="1">
         <v>17</v>
@@ -1513,7 +1519,7 @@
         <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>14</v>
@@ -1586,7 +1592,7 @@
         <v>23</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L9" s="1">
         <v>23</v>
@@ -1689,17 +1695,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2286,8 +2292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2319,7 +2325,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>104</v>
@@ -2330,7 +2336,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>105</v>
@@ -2341,7 +2347,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>105</v>
@@ -2352,7 +2358,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>106</v>
@@ -2363,7 +2369,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>101</v>
@@ -2380,7 +2386,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>107</v>
@@ -2388,7 +2394,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>107</v>
@@ -2396,7 +2402,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>107</v>
@@ -2404,7 +2410,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>107</v>
@@ -2412,17 +2418,17 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2432,10 +2438,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H32"/>
+  <dimension ref="B22:H58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,386 +2450,421 @@
     <col min="8" max="8" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C23" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D23" s="21" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="22">
+    <row r="24" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B24" s="22">
+        <v>4</v>
+      </c>
+      <c r="C24" s="18">
+        <v>4</v>
+      </c>
+      <c r="D24" s="56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="22">
+        <v>4</v>
+      </c>
+      <c r="C28" s="18">
+        <v>1</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="29"/>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="30">
+        <v>4</v>
+      </c>
+      <c r="C32" s="31">
+        <v>2</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="30"/>
+      <c r="C36" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" s="36" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="29"/>
+      <c r="F40" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="G40" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="H40" s="29"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="30">
+        <v>4</v>
+      </c>
+      <c r="C41" s="31">
+        <v>3</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="F41" s="30">
+        <v>4</v>
+      </c>
+      <c r="G41" s="31">
+        <v>3</v>
+      </c>
+      <c r="H41" s="32"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="32"/>
+      <c r="F42" s="30">
         <v>5</v>
       </c>
-      <c r="C2" s="18">
+      <c r="G42" s="31">
+        <v>4</v>
+      </c>
+      <c r="H42" s="32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="30"/>
+      <c r="C43" s="30">
         <v>1</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
+      <c r="D43" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="F43" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="G43" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H43" s="32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="30"/>
+      <c r="C44" s="30">
+        <v>2</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="F44" s="34"/>
+      <c r="G44" s="35">
+        <v>1</v>
+      </c>
+      <c r="H44" s="36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="30"/>
+      <c r="C45" s="30">
+        <v>3</v>
+      </c>
+      <c r="D45" s="32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="30"/>
+      <c r="C46" s="30">
+        <v>4</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="F46" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="G46" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="H5" s="13"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="30">
+      <c r="H46" s="29"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="39"/>
+      <c r="C47" s="39">
         <v>5</v>
       </c>
-      <c r="C6" s="31">
-        <v>2</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" s="13"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="30"/>
-      <c r="C10" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="30" t="s">
+      <c r="D47" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="F47" s="30">
+        <v>4</v>
+      </c>
+      <c r="G47" s="31">
+        <v>3</v>
+      </c>
+      <c r="H47" s="32"/>
+    </row>
+    <row r="48" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="34"/>
+      <c r="C48" s="34">
+        <v>6</v>
+      </c>
+      <c r="D48" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="F48" s="30">
+        <v>5</v>
+      </c>
+      <c r="G48" s="31">
+        <v>6</v>
+      </c>
+      <c r="H48" s="32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="39">
+        <v>7</v>
+      </c>
+      <c r="D49" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="F49" s="30">
+        <v>6</v>
+      </c>
+      <c r="G49" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="H49" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="39">
+        <v>8</v>
+      </c>
+      <c r="D50" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="F50" s="30"/>
+      <c r="G50" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="H50" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F51" s="30">
+        <v>7</v>
+      </c>
+      <c r="G51" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="H51" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F52" s="30"/>
+      <c r="G52" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="29"/>
-      <c r="F14" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="G14" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="H14" s="29"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="30">
-        <v>5</v>
-      </c>
-      <c r="C15" s="31">
-        <v>3</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="F15" s="30">
-        <v>5</v>
-      </c>
-      <c r="G15" s="31">
-        <v>3</v>
-      </c>
-      <c r="H15" s="32"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="D16" s="32"/>
-      <c r="F16" s="30">
-        <v>6</v>
-      </c>
-      <c r="G16" s="31">
-        <v>4</v>
-      </c>
-      <c r="H16" s="32" t="s">
+      <c r="H52" s="38" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="30"/>
-      <c r="C17" s="30">
-        <v>1</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="H17" s="32" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="30"/>
-      <c r="C18" s="30">
-        <v>2</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="35">
-        <v>1</v>
-      </c>
-      <c r="H18" s="36" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="30"/>
-      <c r="C19" s="30">
-        <v>3</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="30"/>
-      <c r="C20" s="30">
-        <v>4</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="G20" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="H20" s="29"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="39"/>
-      <c r="C21" s="39">
-        <v>5</v>
-      </c>
-      <c r="D21" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="F21" s="30">
-        <v>5</v>
-      </c>
-      <c r="G21" s="31">
-        <v>3</v>
-      </c>
-      <c r="H21" s="32"/>
-    </row>
-    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="34"/>
-      <c r="C22" s="34">
-        <v>6</v>
-      </c>
-      <c r="D22" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="F22" s="30">
-        <v>6</v>
-      </c>
-      <c r="G22" s="31">
-        <v>6</v>
-      </c>
-      <c r="H22" s="32" t="s">
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F53" s="30"/>
+      <c r="G53" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="H53" s="38" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="39">
-        <v>7</v>
-      </c>
-      <c r="D23" s="38" t="s">
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F54" s="30">
+        <v>8</v>
+      </c>
+      <c r="G54" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="H54" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="F23" s="30">
-        <v>7</v>
-      </c>
-      <c r="G23" s="31" t="s">
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F55" s="30">
+        <v>9</v>
+      </c>
+      <c r="G55" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="H23" s="32" t="s">
+      <c r="H55" s="32" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="39">
-        <v>8</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="H24" s="32" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F25" s="30">
-        <v>8</v>
-      </c>
-      <c r="G25" s="31" t="s">
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F56" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G56" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="H56" s="38" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F57" s="30">
+        <v>28</v>
+      </c>
+      <c r="G57" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="H25" s="32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F26" s="30"/>
-      <c r="G26" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="H26" s="38" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F27" s="30"/>
-      <c r="G27" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="H27" s="38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F28" s="30">
-        <v>9</v>
-      </c>
-      <c r="G28" s="31" t="s">
+      <c r="H57" s="32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F58" s="34">
+        <v>29</v>
+      </c>
+      <c r="G58" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="H28" s="32" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F29" s="30">
-        <v>10</v>
-      </c>
-      <c r="G29" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="H29" s="32" t="s">
+      <c r="H58" s="36" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F30" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="G30" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="H30" s="38" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F31" s="30">
-        <v>29</v>
-      </c>
-      <c r="G31" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="H31" s="32" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F32" s="34">
-        <v>30</v>
-      </c>
-      <c r="G32" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="H32" s="36" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2848,87 +2889,87 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -2942,7 +2983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2957,12 +2998,12 @@
         <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2971,12 +3012,12 @@
         <v>284</v>
       </c>
       <c r="I2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -2987,7 +3028,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B4">
         <v>68</v>
@@ -2996,7 +3037,7 @@
         <v>9000</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>